<commit_message>
Button presses detected ok.
</commit_message>
<xml_diff>
--- a/src/main/resources/Referee.xlsx
+++ b/src/main/resources/Referee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5FB2B4-C815-4654-8292-BE0D0956A4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8CF0E5-C550-4618-8D0D-716E5EE62388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
   <si>
     <t>pin</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -699,8 +705,8 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
-        <v>11</v>
+      <c r="B8" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>4</v>
@@ -716,8 +722,8 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2">
-        <v>11</v>
+      <c r="B9" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
mqtt messages out ok.
</commit_message>
<xml_diff>
--- a/src/main/resources/Referee.xlsx
+++ b/src/main/resources/Referee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8CF0E5-C550-4618-8D0D-716E5EE62388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26ED61F-4CA8-4020-8BA7-FD678B830A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
@@ -51,18 +51,9 @@
     <t>ON</t>
   </si>
   <si>
-    <t>fop/decisionRequest/A</t>
-  </si>
-  <si>
-    <t>fop/resetDecisions/A</t>
-  </si>
-  <si>
     <t>OFF</t>
   </si>
   <si>
-    <t>fop/startup/A</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
     <t>message</t>
   </si>
   <si>
-    <t>refbox/decision/A</t>
-  </si>
-  <si>
     <t>1 bad</t>
   </si>
   <si>
@@ -132,9 +120,6 @@
     <t>Down light</t>
   </si>
   <si>
-    <t>fop/down/A</t>
-  </si>
-  <si>
     <t>pin action</t>
   </si>
   <si>
@@ -144,9 +129,6 @@
     <t>FLASH</t>
   </si>
   <si>
-    <t>fop/summon/A</t>
-  </si>
-  <si>
     <t>1000 100 50</t>
   </si>
   <si>
@@ -163,6 +145,24 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>fop/decisionRequest</t>
+  </si>
+  <si>
+    <t>fop/summon</t>
+  </si>
+  <si>
+    <t>fop/resetDecisions</t>
+  </si>
+  <si>
+    <t>fop/startup</t>
+  </si>
+  <si>
+    <t>fop/down</t>
+  </si>
+  <si>
+    <t>refbox/decision</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,7 +563,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -572,13 +572,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>1</v>
@@ -587,72 +587,72 @@
         <v>2</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>13</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>4</v>
@@ -663,13 +663,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -683,76 +683,76 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3">
         <v>2</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="3"/>
@@ -760,22 +760,22 @@
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3">
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
@@ -783,17 +783,17 @@
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
         <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -802,13 +802,13 @@
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="9" t="s">
@@ -823,13 +823,13 @@
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3">
         <v>8</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
@@ -846,22 +846,22 @@
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3">
         <v>2</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="3"/>
@@ -869,7 +869,7 @@
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
@@ -882,15 +882,15 @@
         <v>4</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
         <v>6</v>
@@ -903,75 +903,75 @@
         <v>4</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2">
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2">
         <v>5</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>4</v>
@@ -982,13 +982,13 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>4</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
@@ -1002,27 +1002,27 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
         <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2">
         <v>3</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
         <v>3</v>
@@ -1031,15 +1031,15 @@
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
@@ -1048,21 +1048,21 @@
         <v>4</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="9" t="s">
@@ -1077,13 +1077,13 @@
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1">
       <c r="A27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="9" t="s">

</xml_diff>

<commit_message>
Tested with referee config.
</commit_message>
<xml_diff>
--- a/src/main/resources/Referee.xlsx
+++ b/src/main/resources/Referee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26ED61F-4CA8-4020-8BA7-FD678B830A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155BA4C5-115A-48A3-9B56-AE100E4F3873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t>pin</t>
   </si>
@@ -129,9 +129,6 @@
     <t>FLASH</t>
   </si>
   <si>
-    <t>1000 100 50</t>
-  </si>
-  <si>
     <t>1000 200 50</t>
   </si>
   <si>
@@ -163,6 +160,15 @@
   </si>
   <si>
     <t>refbox/decision</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1000 200 200</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -607,7 +613,7 @@
         <v>30</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -618,7 +624,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -627,7 +633,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -638,7 +644,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>5</v>
@@ -652,7 +658,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>4</v>
@@ -669,7 +675,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -689,7 +695,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -698,7 +704,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -706,13 +712,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>11</v>
@@ -723,13 +729,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>13</v>
@@ -743,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3">
         <v>2</v>
@@ -751,8 +757,8 @@
       <c r="E10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>31</v>
+      <c r="F10" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="3"/>
@@ -766,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
@@ -774,8 +780,8 @@
       <c r="E11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>32</v>
+      <c r="F11" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
@@ -789,7 +795,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="9" t="s">
@@ -808,7 +814,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="9" t="s">
@@ -829,7 +835,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
@@ -852,7 +858,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3">
         <v>2</v>
@@ -861,7 +867,7 @@
         <v>30</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="3"/>
@@ -877,12 +883,14 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="G16" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>18</v>
@@ -903,7 +911,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>19</v>
@@ -917,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -926,7 +934,7 @@
         <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -937,16 +945,16 @@
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="2">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -957,7 +965,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>5</v>
@@ -971,7 +979,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>4</v>
@@ -988,7 +996,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
@@ -1004,11 +1012,11 @@
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
-        <v>8</v>
+      <c r="B23" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2">
         <v>3</v>
@@ -1017,7 +1025,7 @@
         <v>30</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1031,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>23</v>
@@ -1048,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>25</v>
@@ -1059,10 +1067,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="9" t="s">
@@ -1080,10 +1088,10 @@
         <v>29</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="9" t="s">

</xml_diff>